<commit_message>
JB & Uses Cases & Scénarios
Mise à jour et ajout
</commit_message>
<xml_diff>
--- a/Journal de bord/Journal de bord.xlsx
+++ b/Journal de bord/Journal de bord.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="27870" windowHeight="12885"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="27870" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,33 @@
   </si>
   <si>
     <t>Un peu complexe</t>
+  </si>
+  <si>
+    <t>Finalisation du Trello</t>
+  </si>
+  <si>
+    <t>Ajout des différents sprint, description etc..</t>
+  </si>
+  <si>
+    <t>Ajout des documents dans Github</t>
+  </si>
+  <si>
+    <t>Création de la maquette + comparaison avec d'autres application</t>
+  </si>
+  <si>
+    <t>ABSENT</t>
+  </si>
+  <si>
+    <t>Premier jet des maquettes</t>
+  </si>
+  <si>
+    <t>Création des uses cases &amp; scénarios</t>
+  </si>
+  <si>
+    <t>Finition des uses cases &amp; scénarios</t>
+  </si>
+  <si>
+    <t>Création d'un Hello World sous Android Studio</t>
   </si>
 </sst>
 </file>
@@ -559,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,51 +758,101 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
+      <c r="A13" s="8">
+        <v>43137</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>43139</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
+      <c r="A15" s="8">
+        <v>43139</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="10">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43139</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="2">
+        <v>9.375E-2</v>
+      </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="8">
+        <v>43139</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="10">
+        <v>3.125E-2</v>
+      </c>
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="8">
+        <v>43139</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="10">
+        <v>6.25E-2</v>
+      </c>
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="8">
+        <v>43139</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="8">
+        <v>43139</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3.125E-2</v>
+      </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -869,7 +946,7 @@
       </c>
       <c r="C35" s="10">
         <f>SUM(C2:C34)</f>
-        <v>0.20833333333333334</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="D35" s="9"/>
     </row>

</xml_diff>